<commit_message>
hopefully adding python tutorial
</commit_message>
<xml_diff>
--- a/sea_level_rise_economics/CGI SLR MIAMI Example.xlsx
+++ b/sea_level_rise_economics/CGI SLR MIAMI Example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfortmann/Google Drive/CGI Modules Updated/Updated SLR Module/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lfortmann/Google Drive/CGI Modules Updated/Complete SLR Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B664E24D-3BB1-4A4F-AD24-8512E4AA00E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D63BF34-1904-9F41-81FE-7B4C583F6E28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="460" windowWidth="27620" windowHeight="14480" xr2:uid="{D13B9AEB-63EA-1143-B588-BD6B0A0A5B75}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="housevalue">'Part 1. MD Tables'!$D$3</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>Part 1: Estimating the expected marginal damages from flooding due to sea level rise</t>
-  </si>
-  <si>
-    <t>Median home value in Region  (in 2017)</t>
   </si>
   <si>
     <t>Table 1. Regional homes exposed to flood and total property values by flood level</t>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>Home count data for flood levels comes from Climate Central Risk Finder Website for Miami, FL</t>
+  </si>
+  <si>
+    <t>Median home value in Region  (in 2012)</t>
   </si>
 </sst>
 </file>
@@ -5510,7 +5510,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5540,7 +5540,7 @@
     </row>
     <row r="3" spans="1:22" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5548,7 +5548,7 @@
         <v>400000</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -5557,7 +5557,7 @@
     </row>
     <row r="6" spans="1:22" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -5571,19 +5571,19 @@
     </row>
     <row r="7" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="9"/>
@@ -5604,19 +5604,19 @@
     </row>
     <row r="8" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="9"/>
@@ -5650,7 +5650,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="12"/>
       <c r="P9" s="15"/>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="22" spans="1:26" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -5912,25 +5912,25 @@
     </row>
     <row r="23" spans="1:26" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="C23" s="77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="77"/>
       <c r="E23" s="78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="78"/>
       <c r="G23" s="77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="77"/>
       <c r="I23" s="78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J23" s="78"/>
       <c r="K23" s="9"/>
@@ -5947,34 +5947,34 @@
     </row>
     <row r="24" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="E24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="F24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="20" t="s">
-        <v>22</v>
-      </c>
       <c r="H24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>22</v>
-      </c>
       <c r="J24" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N24" s="6"/>
       <c r="Q24" s="9"/>
@@ -6391,7 +6391,7 @@
     </row>
     <row r="37" spans="1:16" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
@@ -6407,25 +6407,25 @@
     </row>
     <row r="38" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="C38" s="77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" s="77"/>
       <c r="E38" s="78" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="78"/>
       <c r="G38" s="77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H38" s="77"/>
       <c r="I38" s="78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J38" s="78"/>
       <c r="N38" s="2"/>
@@ -6433,34 +6433,34 @@
     </row>
     <row r="39" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="34" t="s">
+      <c r="D39" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="E39" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="35" t="s">
-        <v>22</v>
-      </c>
       <c r="F39" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="34" t="s">
-        <v>22</v>
-      </c>
       <c r="H39" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I39" s="35" t="s">
-        <v>22</v>
-      </c>
       <c r="J39" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N39" s="2"/>
       <c r="P39"/>
@@ -6896,12 +6896,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6912,19 +6912,19 @@
     <row r="4" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="E5" s="49" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -7139,7 +7139,7 @@
     </row>
     <row r="18" spans="1:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -7150,19 +7150,19 @@
     <row r="19" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="E20" s="49" t="s">
         <v>17</v>
-      </c>
-      <c r="E20" s="49" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -7406,7 +7406,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -7414,13 +7414,13 @@
     </row>
     <row r="3" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="53"/>
       <c r="D3" s="53"/>
       <c r="G3" s="54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -7429,38 +7429,38 @@
     </row>
     <row r="4" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B4" s="79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="79"/>
       <c r="D4" s="79"/>
       <c r="G4" s="49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="C5" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="D5" s="56" t="s">
         <v>35</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>36</v>
       </c>
       <c r="G5" s="12">
         <v>1</v>
@@ -7484,7 +7484,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="58">
         <v>0.01</v>
@@ -7517,7 +7517,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="60">
         <v>0.94</v>
@@ -7550,7 +7550,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="60">
         <v>0.01</v>
@@ -7583,7 +7583,7 @@
     </row>
     <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="61" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="60">
         <v>0.04</v>
@@ -7616,7 +7616,7 @@
     </row>
     <row r="10" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="63">
         <f>SUM(B6:B9)</f>
@@ -7652,7 +7652,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
@@ -7742,7 +7742,7 @@
     </row>
     <row r="16" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -7751,19 +7751,19 @@
     </row>
     <row r="17" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="C17" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="D17" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="E17" s="69" t="s">
         <v>43</v>
-      </c>
-      <c r="E17" s="69" t="s">
-        <v>44</v>
       </c>
       <c r="F17" s="66"/>
     </row>
@@ -7988,7 +7988,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" s="65"/>
       <c r="C28" s="65"/>
@@ -7999,7 +7999,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="65"/>
       <c r="C29" s="65"/>
@@ -8010,7 +8010,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="65" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="65"/>
       <c r="C30" s="65"/>
@@ -8025,7 +8025,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L32" s="17"/>
       <c r="M32" s="17"/>
@@ -8199,62 +8199,62 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="75" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="75" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>